<commit_message>
add strategy amount control
</commit_message>
<xml_diff>
--- a/backtest/rotation_strategy/bt_report/rs_m_ind/single_run/summary.xlsx
+++ b/backtest/rotation_strategy/bt_report/rs_m_ind/single_run/summary.xlsx
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>61477159.42814904</v>
+        <v>61472834.98307132</v>
       </c>
       <c r="C8" s="13" t="n"/>
       <c r="D8" s="13" t="n"/>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>2491.780949052423</v>
+        <v>1769.574371321146</v>
       </c>
       <c r="C9" s="13" t="n"/>
       <c r="D9" s="13" t="n"/>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>5.147715942814904</v>
+        <v>5.147283498307132</v>
       </c>
       <c r="C10" s="13" t="n"/>
       <c r="D10" s="13" t="n"/>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>0.2571234795293944</v>
+        <v>0.2571123371375668</v>
       </c>
       <c r="C11" s="13" t="n"/>
       <c r="D11" s="13" t="n"/>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>6.147715942814904</v>
+        <v>6.147283498307132</v>
       </c>
       <c r="C12" s="13" t="n"/>
       <c r="D12" s="13" t="n"/>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>165.5852141847725</v>
+        <v>165.5941490875089</v>
       </c>
       <c r="C14" s="13" t="n"/>
       <c r="D14" s="13" t="n"/>
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>0.3466994153296191</v>
+        <v>0.2592915258871397</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>0.2027255017202166</v>
+        <v>0.2027283707671999</v>
       </c>
       <c r="C16" s="13" t="n"/>
       <c r="D16" s="13" t="n"/>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1.018600247722466</v>
+        <v>1.018544915964996</v>
       </c>
       <c r="C17" s="13" t="n"/>
       <c r="D17" s="13" t="n"/>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>0.1444474184378625</v>
+        <v>0.1444491273760883</v>
       </c>
       <c r="C18" s="13" t="n"/>
       <c r="D18" s="13" t="n"/>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1.429559963791967</v>
+        <v>1.429485626653772</v>
       </c>
       <c r="C19" s="13" t="n"/>
       <c r="D19" s="13" t="n"/>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>0.2206158238475012</v>
+        <v>0.2206221982536451</v>
       </c>
       <c r="C20" s="13" t="n"/>
       <c r="D20" s="13" t="n"/>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>0.02033799295921488</v>
+        <v>0.02033832807665807</v>
       </c>
       <c r="C21" s="13" t="n"/>
       <c r="D21" s="13" t="n"/>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="B22" s="7" t="n">
-        <v>0.8663097667048713</v>
+        <v>0.8661818613261182</v>
       </c>
       <c r="C22" s="13" t="n"/>
       <c r="D22" s="13" t="n"/>
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="B23" s="7" t="n">
-        <v>0.08179245927151024</v>
+        <v>0.08178311742814071</v>
       </c>
       <c r="C23" s="13" t="n"/>
       <c r="D23" s="13" t="n"/>
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B24" s="7" t="n">
-        <v>0.1942318007741244</v>
+        <v>0.1942205382999752</v>
       </c>
       <c r="C24" s="13" t="n"/>
       <c r="D24" s="13" t="n"/>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="B25" s="7" t="n">
-        <v>0.3831242855589008</v>
+        <v>0.3831267163315676</v>
       </c>
       <c r="C25" s="13" t="n"/>
       <c r="D25" s="13" t="n"/>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B26" s="7" t="n">
-        <v>1.357452207413292</v>
+        <v>1.357357492595406</v>
       </c>
       <c r="C26" s="13" t="n"/>
       <c r="D26" s="13" t="n"/>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B27" s="7" t="n">
-        <v>0.436408168489303</v>
+        <v>0.4363731108430378</v>
       </c>
       <c r="C27" s="13" t="n"/>
       <c r="D27" s="13" t="n"/>
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B28" s="7" t="n">
-        <v>0.5819303150841233</v>
+        <v>0.5819718137654115</v>
       </c>
       <c r="C28" s="13" t="n"/>
       <c r="D28" s="13" t="n"/>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.2533782854074831</v>
+        <v>0.2533796327435372</v>
       </c>
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="13" t="n"/>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>0.1875019601565348</v>
+        <v>0.1874912343484642</v>
       </c>
       <c r="C30" s="13" t="n"/>
       <c r="D30" s="13" t="n"/>
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>0.4091250755557113</v>
+        <v>0.4091223223682925</v>
       </c>
       <c r="C31" s="13" t="n"/>
       <c r="D31" s="13" t="n"/>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>1.009542090483884</v>
+        <v>1.009507203565606</v>
       </c>
       <c r="C32" s="13" t="n"/>
       <c r="D32" s="13" t="n"/>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>1.53654898672668</v>
+        <v>1.536524728143917</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>1.360711467206008</v>
+        <v>1.360663269913359</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>0.03273166980726297</v>
+        <v>0.03273154878383047</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="B36" s="16" t="n">
-        <v>0.1764954329809231</v>
+        <v>0.1765007035881299</v>
       </c>
     </row>
   </sheetData>
@@ -1157,16 +1157,16 @@
         <v>2014</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.6739979999999991</v>
+        <v>0.6740319999999997</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>0.526085147052424</v>
+        <v>0.5261155832367734</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>3.401434552748155</v>
+        <v>3.401419022082913</v>
       </c>
       <c r="E2" s="13" t="n">
-        <v>5.530984444476212</v>
+        <v>5.530934642303164</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>0.5789473684210527</v>
@@ -1177,16 +1177,16 @@
         <v>2015</v>
       </c>
       <c r="B3" s="13" t="n">
-        <v>1.163918953308188</v>
+        <v>1.164001643935123</v>
       </c>
       <c r="C3" s="13" t="n">
-        <v>0.004557541235247292</v>
+        <v>0.004593325340948445</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>2.807094020631129</v>
+        <v>2.807259157457396</v>
       </c>
       <c r="E3" s="13" t="n">
-        <v>3.805933552967469</v>
+        <v>3.806361916300543</v>
       </c>
       <c r="F3" s="13" t="n">
         <v>0.4230769230769231</v>
@@ -1197,16 +1197,16 @@
         <v>2016</v>
       </c>
       <c r="B4" s="13" t="n">
-        <v>-0.07493106772423476</v>
+        <v>-0.07497195390724082</v>
       </c>
       <c r="C4" s="13" t="n">
-        <v>0.1790608455753444</v>
+        <v>0.1790097957669186</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>-0.3880428358917373</v>
+        <v>-0.3882965906471331</v>
       </c>
       <c r="E4" s="13" t="n">
-        <v>-0.002623790174586808</v>
+        <v>-0.002903721554969346</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>0.58</v>
@@ -1217,16 +1217,16 @@
         <v>2017</v>
       </c>
       <c r="B5" s="13" t="n">
-        <v>0.2286561546730114</v>
+        <v>0.2286504920600151</v>
       </c>
       <c r="C5" s="13" t="n">
-        <v>0.3517778150528274</v>
+        <v>0.3517715590122462</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>1.751708929671074</v>
+        <v>1.751679169620282</v>
       </c>
       <c r="E5" s="13" t="n">
-        <v>2.459031597586601</v>
+        <v>2.458992221185023</v>
       </c>
       <c r="F5" s="13" t="n">
         <v>0.6274509803921569</v>
@@ -1237,16 +1237,16 @@
         <v>2018</v>
       </c>
       <c r="B6" s="13" t="n">
-        <v>-0.06164478885452031</v>
+        <v>-0.06164856183473116</v>
       </c>
       <c r="C6" s="13" t="n">
-        <v>0.2451129115074649</v>
+        <v>0.2451092885644754</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>-0.3657431330470629</v>
+        <v>-0.3657508030398334</v>
       </c>
       <c r="E6" s="13" t="n">
-        <v>0.1392502373831807</v>
+        <v>0.1392486684664878</v>
       </c>
       <c r="F6" s="13" t="n">
         <v>0.6470588235294118</v>
@@ -1257,16 +1257,16 @@
         <v>2019</v>
       </c>
       <c r="B7" s="13" t="n">
-        <v>0.3721526890170332</v>
+        <v>0.3721138146567122</v>
       </c>
       <c r="C7" s="13" t="n">
-        <v>-0.07190090715980178</v>
+        <v>-0.07192673756544385</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>1.669872074110096</v>
+        <v>1.669699255603865</v>
       </c>
       <c r="E7" s="13" t="n">
-        <v>0.8531448552839727</v>
+        <v>0.8528096489858246</v>
       </c>
       <c r="F7" s="13" t="n">
         <v>0.4615384615384616</v>
@@ -1277,16 +1277,16 @@
         <v>2020</v>
       </c>
       <c r="B8" s="13" t="n">
-        <v>0.1281152202823918</v>
+        <v>0.1280975583990279</v>
       </c>
       <c r="C8" s="13" t="n">
-        <v>-0.3412861685412383</v>
+        <v>-0.3412950383415547</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>0.6351156579303923</v>
+        <v>0.6350320246848854</v>
       </c>
       <c r="E8" s="13" t="n">
-        <v>-1.788800704481487</v>
+        <v>-1.788924941533658</v>
       </c>
       <c r="F8" s="13" t="n">
         <v>0.3461538461538461</v>
@@ -1297,16 +1297,16 @@
         <v>2021</v>
       </c>
       <c r="B9" s="13" t="n">
-        <v>-0.02762215591571517</v>
+        <v>-0.02765281194445698</v>
       </c>
       <c r="C9" s="13" t="n">
-        <v>-0.1696962702941715</v>
+        <v>-0.1697226802435595</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>-0.05802698326042656</v>
+        <v>-0.05820637044606131</v>
       </c>
       <c r="E9" s="13" t="n">
-        <v>-0.5119944951473883</v>
+        <v>-0.5122191107058666</v>
       </c>
       <c r="F9" s="13" t="n">
         <v>0.4230769230769231</v>
@@ -1317,16 +1317,16 @@
         <v>2022</v>
       </c>
       <c r="B10" s="13" t="n">
-        <v>0.0571952181889997</v>
+        <v>0.05719456833037103</v>
       </c>
       <c r="C10" s="13" t="n">
-        <v>0.2085143383326719</v>
+        <v>0.2085139793681084</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>1.165803160751011</v>
+        <v>1.165725915777688</v>
       </c>
       <c r="E10" s="13" t="n">
-        <v>1.593915405216239</v>
+        <v>1.593822376633312</v>
       </c>
       <c r="F10" s="13" t="n">
         <v>0.52</v>
@@ -1436,28 +1436,28 @@
         <v>-0.0210530000000001</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>0.01218145619732169</v>
+        <v>0.01218145619732192</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>0.02885034595790326</v>
+        <v>0.02885135516999182</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.1116386240152867</v>
+        <v>0.1116385145076799</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.002439842226477085</v>
+        <v>-0.002439840073557575</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>0.05162648550868854</v>
+        <v>0.0516255552823246</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.00183115212861984</v>
+        <v>0.001834516670886188</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.1501881539419969</v>
+        <v>0.1501851307669706</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.2219614621801009</v>
+        <v>0.2219853890131451</v>
       </c>
     </row>
     <row r="3">
@@ -1465,40 +1465,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>0.02261173549789208</v>
+        <v>0.02260828944727411</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>0.1168425971901743</v>
+        <v>0.1168447068980929</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>0.1621127411059444</v>
+        <v>0.1621075964627918</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>0.1397660910836009</v>
+        <v>0.1397208706129209</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>0.1783814009030393</v>
+        <v>0.1784431700518985</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>-0.01796545645864978</v>
+        <v>-0.01793816042874641</v>
       </c>
       <c r="H3" s="15" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.01879267689262742</v>
+        <v>0.01879846898820814</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>0.002218373275552299</v>
+        <v>0.002217568933537528</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>0.1146214888053509</v>
+        <v>0.1146186424393356</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>0.0752650288986132</v>
+        <v>0.07526341716289897</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>0.01011425982083725</v>
+        <v>0.01011704181857409</v>
       </c>
     </row>
     <row r="4">
@@ -1506,40 +1506,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>-0.0884179973696968</v>
+        <v>-0.0884213803977687</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>-0.01717719361947534</v>
+        <v>-0.01717625213033847</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>0.04483374879444413</v>
+        <v>0.04483094037998181</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>-0.05130890299399049</v>
+        <v>-0.05130765394906012</v>
       </c>
       <c r="F4" s="15" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>0.01580243152590532</v>
+        <v>0.01580343696234343</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.02970580629761543</v>
+        <v>0.02967417254858251</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>0.001126064545579952</v>
+        <v>0.001129900184225541</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>-0.02598850265911257</v>
+        <v>-0.02599043370129928</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>0.007268687558289244</v>
+        <v>0.007268799599652098</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>0.03783432463647229</v>
+        <v>0.03783392239085215</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>-0.02302717125740683</v>
+        <v>-0.02303881181491274</v>
       </c>
     </row>
     <row r="5">
@@ -1550,37 +1550,37 @@
         <v>0</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.02615663662358836</v>
+        <v>0.0261547698696567</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.02389275220030385</v>
+        <v>0.02389216261339122</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.001696217933897737</v>
+        <v>0.001696197699624369</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>-0.001924720407990965</v>
+        <v>-0.001924981030898443</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.04775625163709307</v>
+        <v>0.04775654765811033</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.04449089466597322</v>
+        <v>0.04449063502039818</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>0.02581576021450882</v>
+        <v>0.02581416067959319</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>0.01119094116316233</v>
+        <v>0.01119108094408605</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.05986118963084075</v>
+        <v>0.0598605754167072</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>-0.02766513852994246</v>
+        <v>-0.02766487070034152</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>-0.0001597923961645931</v>
+        <v>-0.0001600336483493781</v>
       </c>
     </row>
     <row r="6">
@@ -1588,25 +1588,25 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.008443390326157374</v>
+        <v>0.00844403694235818</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.037557551298812</v>
+        <v>-0.03755764403150197</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>0.007750979664470803</v>
+        <v>0.007744143469604836</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>-0.05467987953267206</v>
+        <v>-0.0546779511685872</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.07040395461897186</v>
+        <v>0.07040382892763253</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>-0.03197431433478259</v>
+        <v>-0.03197414170526169</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.0357907300597059</v>
+        <v>-0.03579129098867173</v>
       </c>
       <c r="I6" s="15" t="n">
         <v>0</v>
@@ -1618,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>0.03434774103576399</v>
+        <v>0.03434809530007055</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>-0.01794369659977235</v>
+        <v>-0.01794334662008856</v>
       </c>
     </row>
     <row r="7">
@@ -1629,40 +1629,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>-0.01260734765549953</v>
+        <v>-0.01260779354165376</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>0.2342286040095154</v>
+        <v>0.2342462503555329</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0.08514031215027651</v>
+        <v>0.08513694936550986</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.001866496562855646</v>
+        <v>0.001864117134826371</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>-0.01272893831933242</v>
+        <v>-0.01272895463545531</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>0.02534363368642167</v>
+        <v>0.02532823850447885</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.01694550854184673</v>
+        <v>-0.01696443838697981</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.009821174755894058</v>
+        <v>0.009820980704160265</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>-0.003252902474748298</v>
+        <v>-0.003251802382334579</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>-0.007299225938378506</v>
+        <v>-0.007298976785700129</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>-0.03849645912347233</v>
+        <v>-0.03850367681299116</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.08327582659004218</v>
+        <v>0.08328008241137907</v>
       </c>
     </row>
     <row r="8">
@@ -1670,40 +1670,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>0.04585212642539838</v>
+        <v>0.04585448488312616</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.09049137488977244</v>
+        <v>-0.09049466225934355</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-0.04592589213914078</v>
+        <v>-0.04592401942410695</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>0.01213693892639944</v>
+        <v>0.01213263332894732</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.01468458756997637</v>
+        <v>0.01468517896695376</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>0.09923237547074604</v>
+        <v>0.09923533102596793</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.05600634270998017</v>
+        <v>0.05601002542445288</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>-0.01631372341156367</v>
+        <v>-0.01628370294090065</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>-0.02262532946454388</v>
+        <v>-0.02262508082538317</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.03838171489589193</v>
+        <v>-0.03838128333925128</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.06691480381499537</v>
+        <v>0.06692646835288807</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.05710400943496241</v>
+        <v>0.05703961406897573</v>
       </c>
     </row>
     <row r="9">
@@ -1711,40 +1711,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>-0.01394309456971088</v>
+        <v>-0.01392941464485675</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>-0.03494211558432825</v>
+        <v>-0.03493618551141442</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>-0.02666093585289975</v>
+        <v>-0.02666933063000809</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>0.02742063807996509</v>
+        <v>0.02737479689474664</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>0.0302386068195668</v>
+        <v>0.03023883651526105</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>-0.0226684575205206</v>
+        <v>-0.02267570253809392</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.009194067170580134</v>
+        <v>0.009184668274411889</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.0199693890661452</v>
+        <v>0.01997322215442998</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.05106434272992155</v>
+        <v>-0.05107101952649096</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>0.01199406487368204</v>
+        <v>0.01200230708452876</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>0.01700257647963976</v>
+        <v>0.01700187169603962</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.00945956220730193</v>
+        <v>0.009473723134998169</v>
       </c>
     </row>
     <row r="10">
@@ -1752,7 +1752,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>-0.0178426271242258</v>
+        <v>-0.01783733780153884</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>0</v>
@@ -1761,16 +1761,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>-0.01472083191364859</v>
+        <v>-0.01472055477557865</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.02577388105029677</v>
+        <v>0.02577571231178655</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>0.07181112352860342</v>
+        <v>0.0718046875906857</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>-0.006323745239896317</v>
+        <v>-0.006325794074340529</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>
@@ -1889,31 +1889,31 @@
         <v/>
       </c>
       <c r="E2" s="15" t="n">
-        <v>0.04331862535215958</v>
+        <v>0.04331869138870825</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>-0.01904821203977047</v>
+        <v>-0.01904821018048075</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>-0.03568555111597804</v>
+        <v>-0.03568454183731373</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.1589128973498108</v>
+        <v>0.15891272533273</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.05998701652159655</v>
+        <v>-0.05998698023864713</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>-0.02812912515648791</v>
+        <v>-0.02812993778888584</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.01975903251994371</v>
+        <v>0.01976246302301332</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.1048161344373812</v>
+        <v>0.1048131137174675</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.2963273490435121</v>
+        <v>0.2963521714147215</v>
       </c>
     </row>
     <row r="3">
@@ -1921,40 +1921,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.1108340626509492</v>
+        <v>-0.1108375396521538</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>-0.02789137400481567</v>
+        <v>-0.02788953591484766</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>-0.04334105364756324</v>
+        <v>-0.04334533373881833</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>-0.07191794627522918</v>
+        <v>-0.07195596670484283</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>-0.0535269744561695</v>
+        <v>-0.05347462733012032</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>0.1831488523326539</v>
+        <v>0.1831784906743321</v>
       </c>
       <c r="H3" s="15" t="n">
         <v>0.08807385286485769</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.2514117738830384</v>
+        <v>0.2514181375592739</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>-0.06648158091713163</v>
+        <v>-0.06648236799820872</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>-0.06827939459584964</v>
+        <v>-0.06828204819045802</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>-0.004360706648024903</v>
+        <v>-0.004361993687415189</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.008673230068610427</v>
+        <v>-0.008670628033343841</v>
       </c>
     </row>
     <row r="4">
@@ -1962,40 +1962,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>0.2005920763378439</v>
+        <v>0.2005879399238613</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>0.02945353442947307</v>
+        <v>0.02945437678863017</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>-0.1321546878515849</v>
+        <v>-0.1321565876960651</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>-0.009751449574708193</v>
+        <v>-0.009750330162947685</v>
       </c>
       <c r="F4" s="15" t="n">
         <v>-0.01869687499886785</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>-0.01723841981023799</v>
+        <v>-0.01723752168006476</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.07813772518755768</v>
+        <v>0.07810503006444258</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.03256465356275962</v>
+        <v>-0.03256098563187182</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>-0.007682305361589536</v>
+        <v>-0.0076842078131798</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>0.001347103425745289</v>
+        <v>0.001347212024823019</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>0.02572114760570154</v>
+        <v>0.0257208551682615</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>0.08276752588950642</v>
+        <v>0.08275464363678875</v>
       </c>
     </row>
     <row r="5">
@@ -2006,37 +2006,37 @@
         <v>0.03685602696773627</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.003952282350411229</v>
+        <v>0.003950462904731333</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.03396792923500569</v>
+        <v>0.03396733935197527</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.0310761039515004</v>
+        <v>0.03107606692474763</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>0.04539433134951087</v>
+        <v>0.0453940587509889</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.01495091784367109</v>
+        <v>0.0149512317467293</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.08960255945622908</v>
+        <v>0.08960227615053706</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>-0.03752450470363822</v>
+        <v>-0.03752599001437007</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>0.001902424317049123</v>
+        <v>0.001902555088135971</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.05668133645517015</v>
+        <v>0.05668072080971998</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>0.02595978116144093</v>
+        <v>0.02596002722889956</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>0.007843777466792323</v>
+        <v>0.007843533214568765</v>
       </c>
     </row>
     <row r="6">
@@ -2044,25 +2044,25 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.01631980569243385</v>
+        <v>0.01632041321633459</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.05397150923450733</v>
+        <v>-0.0539715964214974</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>-0.07366861681359826</v>
+        <v>-0.07367383788494475</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>-0.00822799236567251</v>
+        <v>-0.00822595588923114</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.1062142645608579</v>
+        <v>0.106214131209492</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>0.0437424069815191</v>
+        <v>0.04374257936285342</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.01192638608925289</v>
+        <v>-0.01192694873664324</v>
       </c>
       <c r="I6" s="15" t="n">
         <v>0.07966801273828805</v>
@@ -2074,10 +2074,10 @@
         <v>0.09307593245600398</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>-0.009917403790374202</v>
+        <v>-0.009917055092339311</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.04277175748661421</v>
+        <v>0.04277211227113931</v>
       </c>
     </row>
     <row r="7">
@@ -2085,40 +2085,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>0.003487785091324636</v>
+        <v>0.003487358906415272</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>-0.0126327339247847</v>
+        <v>-0.01261796134591475</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>-0.01712717780748108</v>
+        <v>-0.01713054001444414</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.042912702027462</v>
+        <v>0.04291025026510376</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.0681356139051621</v>
+        <v>0.06813558811331144</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>0.003329291994137451</v>
+        <v>0.003314093194876966</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.05524609546114501</v>
+        <v>-0.05526439884123946</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>-0.01871179378490573</v>
+        <v>-0.01871196860248281</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>-0.01422859211036975</v>
+        <v>-0.01422748577010602</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>-0.03510427704911301</v>
+        <v>-0.03510403766809889</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>-0.035342055723382</v>
+        <v>-0.0353490874411142</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.002404813775539028</v>
+        <v>0.002408870159361642</v>
       </c>
     </row>
     <row r="8">
@@ -2126,40 +2126,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>-0.02525232832629176</v>
+        <v>-0.0252499783336253</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.1564529425427728</v>
+        <v>-0.1564554684398896</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.04863109887605743</v>
+        <v>0.04863307288365593</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>-0.0885570207128864</v>
+        <v>-0.08856084400989672</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.00525950933131103</v>
+        <v>0.005260164443232407</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>-0.06049105636360042</v>
+        <v>-0.060488481045192</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>-0.0817671958730477</v>
+        <v>-0.08176265994509713</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>0.005004886603640513</v>
+        <v>0.005035318857584903</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>0.02997117830149154</v>
+        <v>0.02997143063899466</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.07136387506498965</v>
+        <v>-0.07136347743848137</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.07415576871699581</v>
+        <v>0.07416771882790751</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>-0.06393711308913552</v>
+        <v>-0.06399419313201693</v>
       </c>
     </row>
     <row r="9">
@@ -2167,40 +2167,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>-0.06682627538479924</v>
+        <v>-0.06681293163603441</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>0.03367580378609047</v>
+        <v>0.03368255349837135</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.01694541483409551</v>
+        <v>0.01693722207627513</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>-0.08553960791885229</v>
+        <v>-0.08558081849863908</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>-0.03932797946717559</v>
+        <v>-0.03932881742688477</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>-0.07355538823032548</v>
+        <v>-0.07356214377716108</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.01192254419954897</v>
+        <v>0.01191290009588086</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.08631000181984128</v>
+        <v>0.08631390038068476</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.06355731844030565</v>
+        <v>-0.0635638250399424</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>-0.0217056693948563</v>
+        <v>-0.02169765321332173</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>-0.02620963452639924</v>
+        <v>-0.02621026948517835</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.06051235561164026</v>
+        <v>0.06052720060766759</v>
       </c>
     </row>
     <row r="10">
@@ -2208,7 +2208,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>0.1162683055062594</v>
+        <v>0.1162743664809456</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>0.004280811429914211</v>
@@ -2217,16 +2217,16 @@
         <v>0.07009750317718355</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>0.1142596827268003</v>
+        <v>0.1142600179069098</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>-0.01521045455179715</v>
+        <v>-0.01520865905856217</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>-0.08547366911956455</v>
+        <v>-0.08547898231107232</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.00387268569439736</v>
+        <v>0.003870636859953258</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>

</xml_diff>